<commit_message>
Delete unnecessary files and Adjust and Increased more content
</commit_message>
<xml_diff>
--- a/Plano_de_aula.xlsx
+++ b/Plano_de_aula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29010" windowHeight="12690" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12555" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de aula" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="53">
   <si>
     <t>PLANO DE AULA</t>
   </si>
@@ -145,7 +145,13 @@
     <t>1- Operadores Lógicos</t>
   </si>
   <si>
+    <t>5- O que Javascript Faz?</t>
+  </si>
+  <si>
     <t>2- Operadores Aritméticos</t>
+  </si>
+  <si>
+    <t>6- Cliente x Servidor</t>
   </si>
   <si>
     <t>3- Declaração e uso de Variável e Constante</t>
@@ -190,14 +196,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -245,15 +251,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,9 +289,54 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,23 +351,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,17 +366,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,55 +395,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -420,31 +435,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,151 +501,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,35 +732,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -765,17 +756,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -795,6 +806,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -803,159 +829,154 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1027,55 +1048,57 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Note" xfId="6" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="7" builtinId="11"/>
-    <cellStyle name="Title" xfId="8" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="9" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="10" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="12" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="13" builtinId="19"/>
-    <cellStyle name="Input" xfId="14" builtinId="20"/>
-    <cellStyle name="Output" xfId="15" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="16" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="17" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="18" builtinId="24"/>
-    <cellStyle name="Total" xfId="19" builtinId="25"/>
-    <cellStyle name="Good" xfId="20" builtinId="26"/>
-    <cellStyle name="Bad" xfId="21" builtinId="27"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="60% - Accent6" xfId="2" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="5" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="6" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="7" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="9" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="11" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="15" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="16" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="17" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="18" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="19" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="21" builtinId="29"/>
     <cellStyle name="Neutral" xfId="22" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="23" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="24" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="25" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="26" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="27" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="28" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="29" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="30" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="31" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="32" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="33" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="34" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="35" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="36" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="37" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="38" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="39" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="40" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="41" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="42" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="43" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="44" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="45" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="46" builtinId="52"/>
-    <cellStyle name="Normal 2" xfId="47"/>
+    <cellStyle name="60% - Accent1" xfId="23" builtinId="32"/>
+    <cellStyle name="Bad" xfId="24" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="25" builtinId="42"/>
+    <cellStyle name="Total" xfId="26" builtinId="25"/>
+    <cellStyle name="Output" xfId="27" builtinId="21"/>
+    <cellStyle name="Currency" xfId="28" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="29" builtinId="38"/>
+    <cellStyle name="Note" xfId="30" builtinId="10"/>
+    <cellStyle name="Input" xfId="31" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="32" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="33" builtinId="22"/>
+    <cellStyle name="Good" xfId="34" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="35" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="36" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="37" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="38" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="41" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="42" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
@@ -1449,9 +1472,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
-    <col min="2" max="3" width="48.75" customWidth="1"/>
-    <col min="4" max="4" width="3.25" customWidth="1"/>
+    <col min="1" max="1" width="3.25185185185185" customWidth="1"/>
+    <col min="2" max="3" width="48.7481481481481" customWidth="1"/>
+    <col min="4" max="4" width="3.25185185185185" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1912,15 +1935,15 @@
   </sheetPr>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
-    <col min="2" max="3" width="48.75" customWidth="1"/>
-    <col min="4" max="4" width="3.25" customWidth="1"/>
+    <col min="1" max="1" width="3.25185185185185" customWidth="1"/>
+    <col min="2" max="3" width="48.7481481481481" customWidth="1"/>
+    <col min="4" max="4" width="3.25185185185185" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2073,20 +2096,20 @@
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>31</v>
@@ -2094,7 +2117,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>33</v>
@@ -2106,10 +2129,10 @@
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -2156,10 +2179,10 @@
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:3">
@@ -2206,10 +2229,10 @@
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:3">
@@ -2256,10 +2279,10 @@
     </row>
     <row r="43" spans="2:3">
       <c r="B43" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:3">
@@ -2303,10 +2326,10 @@
     <row r="49" ht="10.5" customHeight="1"/>
     <row r="50" spans="2:3">
       <c r="B50" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="2:3">
@@ -2353,10 +2376,10 @@
     </row>
     <row r="57" spans="2:3">
       <c r="B57" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="2:3">
@@ -2403,10 +2426,10 @@
     </row>
     <row r="64" spans="2:3">
       <c r="B64" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="2:3">
@@ -2453,10 +2476,10 @@
     </row>
     <row r="71" spans="2:3">
       <c r="B71" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="2:3">
@@ -2503,10 +2526,10 @@
     </row>
     <row r="78" spans="2:3">
       <c r="B78" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="2:3">
@@ -2553,10 +2576,10 @@
     </row>
     <row r="85" spans="2:3">
       <c r="B85" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="2:3">

</xml_diff>